<commit_message>
Update translations, user roles
</commit_message>
<xml_diff>
--- a/src/definitions/userroles/userRoles.xlsx
+++ b/src/definitions/userroles/userRoles.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\GitHub\crisiscleanup-web\src\definitions\userroles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FF19EF38-3E58-4FD3-8CA6-548509A83F37}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA10676D-FAF4-4314-9086-59D5CFF0D852}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24750" windowHeight="6615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22500" yWindow="-2730" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="result" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t>inherit</t>
   </si>
@@ -34,9 +34,6 @@
     <t>userRoles.admin_description</t>
   </si>
   <si>
-    <t>portal_admin</t>
-  </si>
-  <si>
     <t>userRoles.portal_admin</t>
   </si>
   <si>
@@ -199,7 +196,25 @@
     <t>x</t>
   </si>
   <si>
-    <t>INSERT INTO public.user_roles(id, name_t, description_t, is_active, create_incident, approve_orgs_full, approve_orgs_preliminary, edit_portal_settings, affiliate_org, invite_workers, remove_workers, phone_agent, advanced_maps, translate, support_agent, crew_management, view_user_contacts, view_sensitive, is_default, level, created_at, updated_at) VALUES</t>
+    <t>invite_orgs</t>
+  </si>
+  <si>
+    <t>portalAdmin</t>
+  </si>
+  <si>
+    <t>INSERT INTO public.user_roles(id, name_t, description_t, is_active, create_incident, approve_orgs_full, approve_orgs_preliminary, edit_portal_settings, affiliate_org, invite_workers, invite_orgs, remove_workers, phone_agent, advanced_maps, translate, support_agent, crew_management, view_user_contacts, view_sensitive, list_order, is_default, level, created_at, updated_at) VALUES</t>
+  </si>
+  <si>
+    <t>list_order</t>
+  </si>
+  <si>
+    <t>incidentAdmin</t>
+  </si>
+  <si>
+    <t>userRoles.incident_admin</t>
+  </si>
+  <si>
+    <t>userRoles.incident_admin_description</t>
   </si>
 </sst>
 </file>
@@ -1041,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA15"/>
+  <dimension ref="A1:AC15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AC10" sqref="AC10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,84 +1067,90 @@
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>44</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>45</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>46</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>47</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>49</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" t="s">
         <v>52</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>53</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>54</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>55</v>
       </c>
-      <c r="X1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>59</v>
+      <c r="AC1" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1170,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="N2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" t="b">
         <v>0</v>
@@ -1179,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="Q2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" t="b">
         <v>1</v>
@@ -1187,44 +1208,50 @@
       <c r="S2" t="b">
         <v>1</v>
       </c>
-      <c r="T2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U2" t="b">
+      <c r="T2" t="b">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
         <v>0</v>
       </c>
       <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
+        <v>10</v>
+      </c>
+      <c r="W2" t="b">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
         <f>LEN(D2)</f>
         <v>15</v>
       </c>
-      <c r="Z2">
+      <c r="AB2">
         <f>LEN(E2)</f>
         <v>27</v>
       </c>
-      <c r="AA2" t="str">
-        <f>"("&amp;A2&amp;", '"&amp;D2&amp;"', '"&amp;E2&amp;"', "&amp;IF(F2,"true","false")&amp;", "&amp;IF(G2,"true","false")&amp;", "&amp;IF(H2,"true","false")&amp;", "&amp;IF(I2,"true","false")&amp;", "&amp;IF(J2,"true","false")&amp;", "&amp;IF(K2,"true","false")&amp;", "&amp;IF(L2,"true","false")&amp;", "&amp;IF(M2,"true","false")&amp;", "&amp;IF(N2,"true","false")&amp;", "&amp;IF(O2,"true","false")&amp;", "&amp;IF(P2,"true","false")&amp;", "&amp;IF(Q2,"true","false")&amp;", "&amp;IF(R2,"true","false")&amp;", "&amp;IF(S2,"true","false")&amp;", '"&amp;T2&amp;"', "&amp;IF(U2,"true","false")&amp;", "&amp;V2&amp;", '"&amp;TEXT(C2,"YYYY-MM-DD")&amp;"', NOW()),"</f>
-        <v>(1, 'userRoles.admin', 'userRoles.admin_description', true, true, true, true, true, true, true, true, false, false, false, true, true, true, 'inherit', false, 0, '2018-05-11', NOW()),</v>
+      <c r="AC2" t="str">
+        <f>"("&amp;A2&amp;", '"&amp;D2&amp;"', '"&amp;E2&amp;"', "&amp;IF(F2,"true","false")&amp;", "&amp;IF(G2,"true","false")&amp;", "&amp;IF(H13,"true","false")&amp;", "&amp;IF(I2,"true","false")&amp;", "&amp;IF(J2,"true","false")&amp;", "&amp;IF(K2,"true","false")&amp;", "&amp;IF(L2,"true","false")&amp;", "&amp;IF(M2,"true","false")&amp;", "&amp;IF(N2,"true","false")&amp;", "&amp;IF(O2,"true","false")&amp;", "&amp;IF(P2,"true","false")&amp;", "&amp;IF(Q2,"true","false")&amp;", "&amp;IF(R2,"true","false")&amp;", "&amp;IF(S2,"true","false")&amp;", "&amp;IF(T2,"true","false")&amp;", '"&amp;U2&amp;"', "&amp;", '"&amp;V2&amp;"', "&amp;IF(W2,"true","false")&amp;", "&amp;X2&amp;", '"&amp;TEXT(C2,"YYYY-MM-DD")&amp;"', NOW()),"</f>
+        <v>(1, 'userRoles.admin', 'userRoles.admin_description', true, true, true, true, true, true, true, true, true, false, false, false, true, true, true, 'inherit', , '10', false, 0, '2018-05-11', NOW()),</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1">
         <v>43231</v>
       </c>
       <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
       <c r="F3" t="b">
         <v>0</v>
       </c>
@@ -1250,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="N3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" t="b">
         <v>0</v>
@@ -1259,7 +1286,7 @@
         <v>0</v>
       </c>
       <c r="Q3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" t="b">
         <v>1</v>
@@ -1267,44 +1294,50 @@
       <c r="S3" t="b">
         <v>1</v>
       </c>
-      <c r="T3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U3" t="b">
+      <c r="T3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
         <v>0</v>
       </c>
       <c r="V3">
-        <v>1</v>
-      </c>
-      <c r="Y3">
-        <f t="shared" ref="Y3:Y12" si="0">LEN(D3)</f>
+        <v>20</v>
+      </c>
+      <c r="W3" t="b">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <f t="shared" ref="AA3:AA13" si="0">LEN(D3)</f>
         <v>22</v>
       </c>
-      <c r="Z3">
-        <f t="shared" ref="Z3:Z12" si="1">LEN(E3)</f>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB13" si="1">LEN(E3)</f>
         <v>34</v>
       </c>
-      <c r="AA3" t="str">
-        <f t="shared" ref="AA3:AA12" si="2">"("&amp;A3&amp;", '"&amp;D3&amp;"', '"&amp;E3&amp;"', "&amp;IF(F3,"true","false")&amp;", "&amp;IF(G3,"true","false")&amp;", "&amp;IF(H3,"true","false")&amp;", "&amp;IF(I3,"true","false")&amp;", "&amp;IF(J3,"true","false")&amp;", "&amp;IF(K3,"true","false")&amp;", "&amp;IF(L3,"true","false")&amp;", "&amp;IF(M3,"true","false")&amp;", "&amp;IF(N3,"true","false")&amp;", "&amp;IF(O3,"true","false")&amp;", "&amp;IF(P3,"true","false")&amp;", "&amp;IF(Q3,"true","false")&amp;", "&amp;IF(R3,"true","false")&amp;", "&amp;IF(S3,"true","false")&amp;", '"&amp;T3&amp;"', "&amp;IF(U3,"true","false")&amp;", "&amp;V3&amp;", '"&amp;TEXT(C3,"YYYY-MM-DD")&amp;"', NOW()),"</f>
-        <v>(2, 'userRoles.portal_admin', 'userRoles.portal_admin_description', false, true, false, true, true, true, true, true, false, false, false, true, true, true, 'inherit', false, 1, '2018-05-11', NOW()),</v>
+      <c r="AC3" t="str">
+        <f t="shared" ref="AC3:AC13" si="2">"("&amp;A3&amp;", '"&amp;D3&amp;"', '"&amp;E3&amp;"', "&amp;IF(F3,"true","false")&amp;", "&amp;IF(G3,"true","false")&amp;", "&amp;IF(H3,"true","false")&amp;", "&amp;IF(I3,"true","false")&amp;", "&amp;IF(J3,"true","false")&amp;", "&amp;IF(K3,"true","false")&amp;", "&amp;IF(L3,"true","false")&amp;", "&amp;IF(M3,"true","false")&amp;", "&amp;IF(N3,"true","false")&amp;", "&amp;IF(O3,"true","false")&amp;", "&amp;IF(P3,"true","false")&amp;", "&amp;IF(Q3,"true","false")&amp;", "&amp;IF(R3,"true","false")&amp;", "&amp;IF(S3,"true","false")&amp;", "&amp;IF(T3,"true","false")&amp;", '"&amp;U3&amp;"', "&amp;IF(W3,"true","false")&amp;", "&amp;X3&amp;", '"&amp;TEXT(C3,"YYYY-MM-DD")&amp;"', NOW()),"</f>
+        <v>(2, 'userRoles.portal_admin', 'userRoles.portal_admin_description', false, true, false, true, true, true, true, true, true, false, false, false, true, true, true, 'inherit', false, 1, '2018-05-11', NOW()),</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>43231</v>
       </c>
       <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
@@ -1330,7 +1363,7 @@
         <v>1</v>
       </c>
       <c r="N4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" t="b">
         <v>0</v>
@@ -1342,49 +1375,55 @@
         <v>0</v>
       </c>
       <c r="R4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" t="b">
         <v>1</v>
       </c>
-      <c r="T4" t="s">
-        <v>0</v>
-      </c>
-      <c r="U4" t="b">
+      <c r="T4" t="b">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
         <v>0</v>
       </c>
       <c r="V4">
+        <v>40</v>
+      </c>
+      <c r="W4" t="b">
+        <v>0</v>
+      </c>
+      <c r="X4">
         <v>2</v>
       </c>
-      <c r="Y4">
+      <c r="AA4">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="Z4">
+      <c r="AB4">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="AA4" t="str">
+      <c r="AC4" t="str">
         <f t="shared" si="2"/>
-        <v>(3, 'userRoles.primary_contact', 'userRoles.primary_contact_description', true, false, false, false, false, true, true, true, false, false, false, false, true, true, 'inherit', false, 2, '2018-05-11', NOW()),</v>
+        <v>(3, 'userRoles.primary_contact', 'userRoles.primary_contact_description', true, false, false, false, false, true, true, true, true, false, false, false, false, true, true, 'inherit', false, 2, '2018-05-11', NOW()),</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
         <v>43315</v>
       </c>
       <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
@@ -1410,7 +1449,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" t="b">
         <v>0</v>
@@ -1422,49 +1461,55 @@
         <v>0</v>
       </c>
       <c r="R5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" t="b">
         <v>1</v>
       </c>
-      <c r="T5" t="s">
-        <v>0</v>
-      </c>
-      <c r="U5" t="b">
+      <c r="T5" t="b">
+        <v>1</v>
+      </c>
+      <c r="U5" t="s">
         <v>0</v>
       </c>
       <c r="V5">
+        <v>50</v>
+      </c>
+      <c r="W5" t="b">
+        <v>0</v>
+      </c>
+      <c r="X5">
         <v>3</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="Z5">
+      <c r="AB5">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="AA5" t="str">
+      <c r="AC5" t="str">
         <f t="shared" si="2"/>
-        <v>(4, 'userRoles.incident_primary_contact', 'userRoles.incident_primary_contact_description', true, false, false, false, false, true, true, true, false, false, false, false, true, true, 'inherit', false, 3, '2018-08-03', NOW()),</v>
+        <v>(4, 'userRoles.incident_primary_contact', 'userRoles.incident_primary_contact_description', true, false, false, false, false, true, true, true, true, false, false, false, false, true, true, 'inherit', false, 3, '2018-08-03', NOW()),</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>43231</v>
       </c>
       <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
@@ -1490,7 +1535,7 @@
         <v>1</v>
       </c>
       <c r="N6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" t="b">
         <v>0</v>
@@ -1499,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="Q6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6" t="b">
         <v>1</v>
@@ -1507,44 +1552,50 @@
       <c r="S6" t="b">
         <v>1</v>
       </c>
-      <c r="T6" t="s">
-        <v>0</v>
-      </c>
-      <c r="U6" t="b">
+      <c r="T6" t="b">
+        <v>1</v>
+      </c>
+      <c r="U6" t="s">
         <v>0</v>
       </c>
       <c r="V6">
+        <v>60</v>
+      </c>
+      <c r="W6" t="b">
+        <v>0</v>
+      </c>
+      <c r="X6">
         <v>3</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="Z6">
+      <c r="AB6">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="AA6" t="str">
+      <c r="AC6" t="str">
         <f t="shared" si="2"/>
-        <v>(5, 'userRoles.team_leader', 'userRoles.team_leader_description', true, false, false, false, false, false, true, true, false, false, false, true, true, true, 'inherit', false, 3, '2018-05-11', NOW()),</v>
+        <v>(5, 'userRoles.team_leader', 'userRoles.team_leader_description', true, false, false, false, false, false, true, true, true, false, false, false, true, true, true, 'inherit', false, 3, '2018-05-11', NOW()),</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1">
         <v>43231</v>
       </c>
       <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
@@ -1570,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="N7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" t="b">
         <v>0</v>
@@ -1579,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="Q7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7" t="b">
         <v>1</v>
@@ -1587,44 +1638,50 @@
       <c r="S7" t="b">
         <v>1</v>
       </c>
-      <c r="T7" t="s">
-        <v>0</v>
-      </c>
-      <c r="U7" t="b">
-        <v>1</v>
+      <c r="T7" t="b">
+        <v>1</v>
+      </c>
+      <c r="U7" t="s">
+        <v>0</v>
       </c>
       <c r="V7">
+        <v>70</v>
+      </c>
+      <c r="W7" t="b">
+        <v>1</v>
+      </c>
+      <c r="X7">
         <v>3</v>
       </c>
-      <c r="Y7">
+      <c r="AA7">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="Z7">
+      <c r="AB7">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="AA7" t="str">
+      <c r="AC7" t="str">
         <f t="shared" si="2"/>
-        <v>(6, 'userRoles.worker', 'userRoles.worker_description', true, false, false, false, false, false, true, true, false, false, false, true, true, true, 'inherit', true, 3, '2018-05-11', NOW()),</v>
+        <v>(6, 'userRoles.worker', 'userRoles.worker_description', true, false, false, false, false, false, true, true, true, false, false, false, true, true, true, 'inherit', true, 3, '2018-05-11', NOW()),</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1">
         <v>43231</v>
       </c>
       <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
       <c r="F8" t="b">
         <v>0</v>
       </c>
@@ -1653,58 +1710,64 @@
         <v>1</v>
       </c>
       <c r="O8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="b">
         <v>1</v>
       </c>
       <c r="R8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8" t="b">
         <v>0</v>
       </c>
-      <c r="T8" t="s">
-        <v>0</v>
-      </c>
-      <c r="U8" t="b">
+      <c r="T8" t="b">
+        <v>0</v>
+      </c>
+      <c r="U8" t="s">
         <v>0</v>
       </c>
       <c r="V8">
+        <v>80</v>
+      </c>
+      <c r="W8" t="b">
+        <v>0</v>
+      </c>
+      <c r="X8">
         <v>3</v>
       </c>
-      <c r="Y8">
+      <c r="AA8">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="Z8">
+      <c r="AB8">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="AA8" t="str">
+      <c r="AC8" t="str">
         <f t="shared" si="2"/>
-        <v>(7, 'userRoles.phone_agent', 'userRoles.phone_agent_description', false, false, false, false, false, false, true, true, true, false, true, true, false, false, 'inherit', false, 3, '2018-05-11', NOW()),</v>
+        <v>(7, 'userRoles.phone_agent', 'userRoles.phone_agent_description', false, false, false, false, false, false, true, true, true, true, false, true, true, false, false, 'inherit', false, 3, '2018-05-11', NOW()),</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1">
         <v>43231</v>
       </c>
       <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
       <c r="F9" t="b">
         <v>0</v>
       </c>
@@ -1730,61 +1793,67 @@
         <v>1</v>
       </c>
       <c r="N9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9" t="b">
-        <v>1</v>
-      </c>
-      <c r="T9" t="s">
-        <v>0</v>
-      </c>
-      <c r="U9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T9" t="b">
+        <v>1</v>
+      </c>
+      <c r="U9" t="s">
         <v>0</v>
       </c>
       <c r="V9">
+        <v>90</v>
+      </c>
+      <c r="W9" t="b">
+        <v>0</v>
+      </c>
+      <c r="X9">
         <v>3</v>
       </c>
-      <c r="Y9">
+      <c r="AA9">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="Z9">
+      <c r="AB9">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="AA9" t="str">
+      <c r="AC9" t="str">
         <f t="shared" si="2"/>
-        <v>(8, 'userRoles.map_specialist', 'userRoles.map_specialist_description', false, false, false, false, false, false, true, true, false, true, false, true, false, true, 'inherit', false, 3, '2018-05-11', NOW()),</v>
+        <v>(8, 'userRoles.map_specialist', 'userRoles.map_specialist_description', false, false, false, false, false, false, true, true, true, false, true, false, true, false, true, 'inherit', false, 3, '2018-05-11', NOW()),</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1">
         <v>43231</v>
       </c>
       <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
         <v>26</v>
       </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
@@ -1810,61 +1879,67 @@
         <v>1</v>
       </c>
       <c r="N10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10" t="b">
         <v>0</v>
       </c>
       <c r="P10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="b">
         <v>1</v>
       </c>
       <c r="R10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10" t="b">
-        <v>1</v>
-      </c>
-      <c r="T10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U10" t="b">
+        <v>0</v>
+      </c>
+      <c r="T10" t="b">
+        <v>1</v>
+      </c>
+      <c r="U10" t="s">
         <v>0</v>
       </c>
       <c r="V10">
+        <v>100</v>
+      </c>
+      <c r="W10" t="b">
+        <v>0</v>
+      </c>
+      <c r="X10">
         <v>3</v>
       </c>
-      <c r="Y10">
+      <c r="AA10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="Z10">
+      <c r="AB10">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="AA10" t="str">
+      <c r="AC10" t="str">
         <f t="shared" si="2"/>
-        <v>(9, 'userRoles.translator', 'userRoles.translator_description', false, false, false, false, false, false, true, true, false, false, true, true, false, true, 'inherit', false, 3, '2018-05-11', NOW()),</v>
+        <v>(9, 'userRoles.translator', 'userRoles.translator_description', false, false, false, false, false, false, true, true, true, false, false, true, true, false, true, 'inherit', false, 3, '2018-05-11', NOW()),</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1">
         <v>43231</v>
       </c>
       <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
         <v>29</v>
       </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
@@ -1890,7 +1965,7 @@
         <v>1</v>
       </c>
       <c r="N11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" t="b">
         <v>0</v>
@@ -1899,119 +1974,217 @@
         <v>0</v>
       </c>
       <c r="Q11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11" t="b">
-        <v>1</v>
-      </c>
-      <c r="T11" t="s">
-        <v>0</v>
-      </c>
-      <c r="U11" t="b">
+        <v>0</v>
+      </c>
+      <c r="T11" t="b">
+        <v>1</v>
+      </c>
+      <c r="U11" t="s">
         <v>0</v>
       </c>
       <c r="V11">
+        <v>110</v>
+      </c>
+      <c r="W11" t="b">
+        <v>0</v>
+      </c>
+      <c r="X11">
         <v>3</v>
       </c>
-      <c r="Y11">
+      <c r="AA11">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="Z11">
+      <c r="AB11">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="AA11" t="str">
+      <c r="AC11" t="str">
         <f t="shared" si="2"/>
-        <v>(10, 'userRoles.support_agent', 'userRoles.support_agent_description', false, false, false, false, false, false, true, true, false, false, false, true, false, true, 'inherit', false, 3, '2018-05-11', NOW()),</v>
+        <v>(10, 'userRoles.support_agent', 'userRoles.support_agent_description', false, false, false, false, false, false, true, true, true, false, false, false, true, false, true, 'inherit', false, 3, '2018-05-11', NOW()),</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1">
         <v>43231</v>
       </c>
       <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
         <v>32</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U12" t="s">
         <v>33</v>
       </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12" t="b">
-        <v>0</v>
-      </c>
-      <c r="O12" t="b">
-        <v>0</v>
-      </c>
-      <c r="P12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="b">
-        <v>0</v>
-      </c>
-      <c r="R12" t="b">
-        <v>1</v>
-      </c>
-      <c r="S12" t="b">
-        <v>1</v>
-      </c>
-      <c r="T12" t="s">
-        <v>34</v>
-      </c>
-      <c r="U12" t="b">
-        <v>0</v>
-      </c>
       <c r="V12">
+        <v>120</v>
+      </c>
+      <c r="W12" t="b">
+        <v>0</v>
+      </c>
+      <c r="X12">
         <v>4</v>
       </c>
-      <c r="Y12">
+      <c r="AA12">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="Z12">
+      <c r="AB12">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="AA12" t="str">
+      <c r="AC12" t="str">
         <f t="shared" si="2"/>
-        <v>(11, 'userRoles.guest_worker', 'userRoles.guest_worker_description', false, false, false, false, false, false, false, false, false, false, false, false, true, true, 'redactDigits', false, 4, '2018-05-11', NOW()),</v>
+        <v>(11, 'userRoles.guest_worker', 'userRoles.guest_worker_description', false, false, false, false, false, false, false, false, false, false, false, false, false, true, true, 'redactDigits', false, 4, '2018-05-11', NOW()),</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="Y15">
-        <f>MAX(Y2:Z12)</f>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="1">
+        <v>43511</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" t="b">
+        <v>0</v>
+      </c>
+      <c r="P13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" t="b">
+        <v>1</v>
+      </c>
+      <c r="S13" t="b">
+        <v>1</v>
+      </c>
+      <c r="T13" t="b">
+        <v>1</v>
+      </c>
+      <c r="U13" t="s">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>30</v>
+      </c>
+      <c r="W13" t="b">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="AC13" t="str">
+        <f t="shared" si="2"/>
+        <v>(12, 'userRoles.incident_admin', 'userRoles.incident_admin_description', false, false, true, true, false, true, true, true, true, false, false, false, true, true, true, 'inherit', false, 1, '2019-02-15', NOW()),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AA15">
+        <f>MAX(AA2:AB12)</f>
         <v>46</v>
       </c>
     </row>

</xml_diff>